<commit_message>
replaced %in% with base::merge
</commit_message>
<xml_diff>
--- a/data/comtrade_total_exports_2021M.xlsx
+++ b/data/comtrade_total_exports_2021M.xlsx
@@ -2353,7 +2353,7 @@
         <v>44197</v>
       </c>
       <c r="B111">
-        <v>2536387816.336</v>
+        <v>2965813121.872</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -4477,7 +4477,7 @@
         <v>44228</v>
       </c>
       <c r="B229">
-        <v>2717261987.91</v>
+        <v>2921212300.724</v>
       </c>
       <c r="C229" t="inlineStr">
         <is>
@@ -6601,7 +6601,7 @@
         <v>44256</v>
       </c>
       <c r="B347">
-        <v>3430289300.038</v>
+        <v>3805193396.882</v>
       </c>
       <c r="C347" t="inlineStr">
         <is>
@@ -8707,7 +8707,7 @@
         <v>44287</v>
       </c>
       <c r="B464">
-        <v>2915646561.545</v>
+        <v>3199733948.669</v>
       </c>
       <c r="C464" t="inlineStr">
         <is>
@@ -10813,7 +10813,7 @@
         <v>44317</v>
       </c>
       <c r="B581">
-        <v>3137973188.198</v>
+        <v>3393551859.085</v>
       </c>
       <c r="C581" t="inlineStr">
         <is>
@@ -12919,7 +12919,7 @@
         <v>44348</v>
       </c>
       <c r="B698">
-        <v>3644161461.983</v>
+        <v>3876518214.218</v>
       </c>
       <c r="C698" t="inlineStr">
         <is>
@@ -15025,7 +15025,7 @@
         <v>44378</v>
       </c>
       <c r="B815">
-        <v>2958716131.923</v>
+        <v>3157199563.08</v>
       </c>
       <c r="C815" t="inlineStr">
         <is>
@@ -17131,7 +17131,7 @@
         <v>44409</v>
       </c>
       <c r="B932">
-        <v>3279103225.71</v>
+        <v>3577164738.589</v>
       </c>
       <c r="C932" t="inlineStr">
         <is>
@@ -19237,7 +19237,7 @@
         <v>44440</v>
       </c>
       <c r="B1049">
-        <v>3469309587.383</v>
+        <v>3683539147.36</v>
       </c>
       <c r="C1049" t="inlineStr">
         <is>
@@ -21343,7 +21343,7 @@
         <v>44470</v>
       </c>
       <c r="B1166">
-        <v>3776281916.454</v>
+        <v>4157701042.656</v>
       </c>
       <c r="C1166" t="inlineStr">
         <is>
@@ -23449,7 +23449,7 @@
         <v>44501</v>
       </c>
       <c r="B1283">
-        <v>4495170553.346</v>
+        <v>4605525576.116</v>
       </c>
       <c r="C1283" t="inlineStr">
         <is>
@@ -25555,7 +25555,7 @@
         <v>44531</v>
       </c>
       <c r="B1400">
-        <v>4336362238.886</v>
+        <v>4293699080.01</v>
       </c>
       <c r="C1400" t="inlineStr">
         <is>

</xml_diff>